<commit_message>
Replace Group2 todo list with latest
</commit_message>
<xml_diff>
--- a/GROUP_NOTES/Group2_TodoList.xlsx
+++ b/GROUP_NOTES/Group2_TodoList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mreth\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/989c3ab304c45128/Desktop/331_Final_Project-main/GROUP_NOTES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9656EB2-2823-43EA-8C38-25ADD5E4E238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{C9656EB2-2823-43EA-8C38-25ADD5E4E238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E5AAE0A-A64A-4514-AA73-11DB9A02D852}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adrian Angeles" sheetId="1" r:id="rId1"/>
@@ -1115,20 +1115,20 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.140625" customWidth="1"/>
+    <col min="1" max="1" width="1.125" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.125" customWidth="1"/>
+    <col min="4" max="4" width="15.75" customWidth="1"/>
+    <col min="5" max="5" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:8" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1139,8 +1139,8 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
@@ -1153,7 +1153,7 @@
       <c r="G3" s="11"/>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
@@ -1166,8 +1166,8 @@
       <c r="G4" s="14"/>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="16" t="s">
         <v>3</v>
       </c>
@@ -1178,7 +1178,7 @@
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
     </row>
-    <row r="7" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="3">
         <v>1</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="3">
         <v>1</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1268,7 +1268,7 @@
       </c>
       <c r="H10"/>
     </row>
-    <row r="11" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <v>1</v>
       </c>
@@ -1289,7 +1289,7 @@
       </c>
       <c r="H11"/>
     </row>
-    <row r="12" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <v>1</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <v>1</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <v>1</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="3"/>
       <c r="C15"/>
       <c r="D15" s="6"/>
@@ -1365,7 +1365,7 @@
       <c r="G15" s="4"/>
       <c r="H15"/>
     </row>
-    <row r="16" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="3"/>
       <c r="C16"/>
       <c r="D16"/>
@@ -1427,17 +1427,17 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="6" max="6" width="53.5703125" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.75" customWidth="1"/>
+    <col min="2" max="2" width="15.75" customWidth="1"/>
+    <col min="3" max="4" width="30.75" customWidth="1"/>
+    <col min="5" max="5" width="22.375" customWidth="1"/>
+    <col min="6" max="6" width="53.625" customWidth="1"/>
+    <col min="7" max="7" width="2.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:8" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1448,8 +1448,8 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
@@ -1462,7 +1462,7 @@
       <c r="G3" s="11"/>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
@@ -1475,8 +1475,8 @@
       <c r="G4" s="14"/>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="16" t="s">
         <v>3</v>
       </c>
@@ -1487,7 +1487,7 @@
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
     </row>
-    <row r="7" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="3">
         <v>1</v>
       </c>
@@ -1531,7 +1531,7 @@
       </c>
       <c r="H8"/>
     </row>
-    <row r="9" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="3">
         <v>0.75</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>0.5</v>
       </c>
@@ -1575,7 +1575,7 @@
       </c>
       <c r="H10"/>
     </row>
-    <row r="11" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <v>0.25</v>
       </c>
@@ -1596,7 +1596,7 @@
       </c>
       <c r="H11"/>
     </row>
-    <row r="12" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <v>0</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <v>0</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <v>0</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <v>0</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
@@ -1750,17 +1750,17 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="4" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.75" customWidth="1"/>
+    <col min="2" max="2" width="15.75" customWidth="1"/>
+    <col min="3" max="4" width="30.75" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="53.5703125" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" customWidth="1"/>
+    <col min="6" max="6" width="53.625" customWidth="1"/>
+    <col min="7" max="7" width="2.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:8" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1771,8 +1771,8 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
@@ -1785,7 +1785,7 @@
       <c r="G3" s="11"/>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
@@ -1798,8 +1798,8 @@
       <c r="G4" s="14"/>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="16" t="s">
         <v>3</v>
       </c>
@@ -1810,7 +1810,7 @@
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
     </row>
-    <row r="7" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="3">
         <v>1</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="3">
         <v>0.75</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>0.5</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <v>0.25</v>
       </c>
@@ -1923,7 +1923,7 @@
       </c>
       <c r="H11"/>
     </row>
-    <row r="12" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <v>0</v>
       </c>
@@ -1944,7 +1944,7 @@
       </c>
       <c r="H12"/>
     </row>
-    <row r="13" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <v>0</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <v>0</v>
       </c>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="H14"/>
     </row>
-    <row r="15" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <v>0</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
@@ -2065,23 +2065,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30E5B4F-2070-4E52-85B8-76686C2B4348}">
   <dimension ref="B1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="53.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="44.85546875" customWidth="1"/>
+    <col min="1" max="1" width="2.75" customWidth="1"/>
+    <col min="2" max="2" width="15.75" customWidth="1"/>
+    <col min="3" max="3" width="30.75" customWidth="1"/>
+    <col min="4" max="4" width="23.625" customWidth="1"/>
+    <col min="5" max="5" width="15.75" customWidth="1"/>
+    <col min="6" max="6" width="53.625" customWidth="1"/>
+    <col min="7" max="7" width="10.125" customWidth="1"/>
+    <col min="8" max="8" width="44.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:8" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2092,8 +2092,8 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
@@ -2106,7 +2106,7 @@
       <c r="G3" s="11"/>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
@@ -2119,8 +2119,8 @@
       <c r="G4" s="14"/>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="16" t="s">
         <v>3</v>
       </c>
@@ -2131,7 +2131,7 @@
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
     </row>
-    <row r="7" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="3">
         <v>1</v>
       </c>
@@ -2162,13 +2162,13 @@
         <v>4</v>
       </c>
       <c r="D8" s="6">
-        <v>45943</v>
+        <v>46001</v>
       </c>
       <c r="E8" s="6">
-        <v>45943</v>
+        <v>46004</v>
       </c>
       <c r="F8" s="4">
-        <v>45943</v>
+        <v>46004</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>21</v>
@@ -2177,7 +2177,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="3">
         <v>1</v>
       </c>
@@ -2185,13 +2185,13 @@
         <v>5</v>
       </c>
       <c r="D9" s="6">
-        <v>45943</v>
+        <v>46002</v>
       </c>
       <c r="E9" s="6">
-        <v>45943</v>
+        <v>46004</v>
       </c>
       <c r="F9" s="4">
-        <v>45943</v>
+        <v>46004</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>21</v>
@@ -2200,7 +2200,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -2208,13 +2208,13 @@
         <v>30</v>
       </c>
       <c r="D10" s="6">
-        <v>45944</v>
+        <v>46005</v>
       </c>
       <c r="E10" s="6">
-        <v>45944</v>
+        <v>46005</v>
       </c>
       <c r="F10" s="4">
-        <v>45944</v>
+        <v>46005</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>27</v>
@@ -2223,7 +2223,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <v>1</v>
       </c>
@@ -2231,20 +2231,20 @@
         <v>36</v>
       </c>
       <c r="D11" s="6">
-        <v>45944</v>
+        <v>46005</v>
       </c>
       <c r="E11" s="6">
-        <v>45944</v>
+        <v>46005</v>
       </c>
       <c r="F11" s="4">
-        <v>45944</v>
+        <v>46005</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>27</v>
       </c>
       <c r="H11"/>
     </row>
-    <row r="12" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <v>1</v>
       </c>
@@ -2252,13 +2252,13 @@
         <v>39</v>
       </c>
       <c r="D12" s="6">
-        <v>45945</v>
+        <v>46006</v>
       </c>
       <c r="E12" s="6">
-        <v>45945</v>
+        <v>46006</v>
       </c>
       <c r="F12" s="4">
-        <v>45945</v>
+        <v>46006</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>27</v>
@@ -2267,7 +2267,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <v>1</v>
       </c>
@@ -2275,13 +2275,13 @@
         <v>40</v>
       </c>
       <c r="D13" s="6">
-        <v>45945</v>
+        <v>46006</v>
       </c>
       <c r="E13" s="6">
-        <v>45945</v>
+        <v>46006</v>
       </c>
       <c r="F13" s="4">
-        <v>45945</v>
+        <v>46006</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>27</v>
@@ -2290,7 +2290,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <v>1</v>
       </c>
@@ -2298,13 +2298,13 @@
         <v>42</v>
       </c>
       <c r="D14" s="6">
-        <v>45946</v>
+        <v>46007</v>
       </c>
       <c r="E14" s="6">
-        <v>45946</v>
+        <v>46007</v>
       </c>
       <c r="F14" s="4">
-        <v>45946</v>
+        <v>46007</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>27</v>
@@ -2313,7 +2313,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <v>1</v>
       </c>
@@ -2321,13 +2321,13 @@
         <v>33</v>
       </c>
       <c r="D15" s="6">
-        <v>45947</v>
+        <v>46007</v>
       </c>
       <c r="E15" s="6">
-        <v>45946</v>
+        <v>46007</v>
       </c>
       <c r="F15" s="4">
-        <v>45947</v>
+        <v>46007</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>27</v>
@@ -2336,7 +2336,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>

</xml_diff>

<commit_message>
Update Group2 todo list
</commit_message>
<xml_diff>
--- a/GROUP_NOTES/Group2_TodoList.xlsx
+++ b/GROUP_NOTES/Group2_TodoList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/989c3ab304c45128/Desktop/331_Final_Project-main/GROUP_NOTES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{C9656EB2-2823-43EA-8C38-25ADD5E4E238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E5AAE0A-A64A-4514-AA73-11DB9A02D852}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{C9656EB2-2823-43EA-8C38-25ADD5E4E238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A2C63A2-CC78-4AF4-9974-74F0647C83C5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5376" yWindow="3540" windowWidth="24336" windowHeight="9696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adrian Angeles" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="35">
   <si>
     <t>To-do list</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Preparation</t>
   </si>
   <si>
-    <t>Hand-off</t>
-  </si>
-  <si>
     <t>% done</t>
   </si>
   <si>
@@ -91,126 +88,39 @@
     <t>Name: Adrian Angeles</t>
   </si>
   <si>
-    <t>Date: 10/17/25</t>
-  </si>
-  <si>
     <t>Name: Ali Mustafa</t>
   </si>
   <si>
     <t>Name: Mret Hein</t>
   </si>
   <si>
-    <t>Date: 10/17</t>
-  </si>
-  <si>
     <t>Name: Aditya Dwivedi</t>
   </si>
   <si>
     <t>1 Day</t>
   </si>
   <si>
-    <t>Create Queries</t>
-  </si>
-  <si>
-    <t>Create Markdown</t>
-  </si>
-  <si>
-    <t>Feedback Session</t>
-  </si>
-  <si>
-    <t>Pair Recording Session</t>
-  </si>
-  <si>
-    <t>2 Days</t>
-  </si>
-  <si>
     <t>1Day</t>
   </si>
   <si>
-    <t>Set up Initial Meeting</t>
-  </si>
-  <si>
-    <t>2nd Group Meeting</t>
-  </si>
-  <si>
     <t>Query Creation</t>
   </si>
   <si>
-    <t>Markdown Creaton</t>
-  </si>
-  <si>
-    <t>Set Up 2nd Meeting</t>
-  </si>
-  <si>
     <t>Pair Recording</t>
   </si>
   <si>
-    <t>Combine Videos</t>
-  </si>
-  <si>
-    <t>Update Github Repo</t>
-  </si>
-  <si>
     <t>Markdown Creation</t>
   </si>
   <si>
-    <t>Gather Individual Files</t>
-  </si>
-  <si>
-    <t>Submission</t>
-  </si>
-  <si>
     <t>Error Assistance</t>
   </si>
   <si>
     <t>Format Review</t>
   </si>
   <si>
-    <t>Assist With Charts</t>
-  </si>
-  <si>
     <t>FeedBack Session</t>
   </si>
   <si>
-    <t>Took Video Editing Role</t>
-  </si>
-  <si>
-    <t>Set up Editing Environment</t>
-  </si>
-  <si>
-    <t>Assist in Todo lists and Update Gantt Chart</t>
-  </si>
-  <si>
-    <t>Set Up The 2nd Peer Review Meeting</t>
-  </si>
-  <si>
-    <t>Delegated Tasks</t>
-  </si>
-  <si>
-    <t>Check Up On Members</t>
-  </si>
-  <si>
-    <t>1DDay</t>
-  </si>
-  <si>
-    <t>1D</t>
-  </si>
-  <si>
-    <t>Join The Individual Videos together</t>
-  </si>
-  <si>
-    <t>Assigned Tasks to each Member</t>
-  </si>
-  <si>
-    <t>2Day</t>
-  </si>
-  <si>
-    <t>Gave Feedback to Others</t>
-  </si>
-  <si>
-    <t>Set up call on Discord</t>
-  </si>
-  <si>
     <t>Helped Brainstorm Ideas and Areas that Needed Improvement</t>
   </si>
   <si>
@@ -226,31 +136,16 @@
     <t>Helped Offer Solutions to Problems</t>
   </si>
   <si>
-    <t>Created Gantt Chart</t>
-  </si>
-  <si>
-    <t>Prepared Tools Needed to Edit Videos</t>
-  </si>
-  <si>
-    <t>Created a Google Meeting for recording</t>
-  </si>
-  <si>
-    <t>Handed In the Combined Video</t>
-  </si>
-  <si>
-    <t>Created New Section on the Repository for the Assignment</t>
-  </si>
-  <si>
-    <t>Checked In on Progress</t>
-  </si>
-  <si>
-    <t>Updated the Repository and Submit every File Needed</t>
-  </si>
-  <si>
     <t>Helped check the group's queries use set operators</t>
   </si>
   <si>
     <t xml:space="preserve">Decided on doing a double take </t>
+  </si>
+  <si>
+    <t>Date: 12/16</t>
+  </si>
+  <si>
+    <t>Date: 12/16/25</t>
   </si>
 </sst>
 </file>
@@ -406,7 +301,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -424,12 +319,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="4">
@@ -464,7 +353,7 @@
     <cellStyle name="Percent" xfId="5" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="23">
     <dxf>
       <font>
         <b val="0"/>
@@ -514,6 +403,12 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -536,6 +431,165 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Perpetua"/>
+        <family val="1"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Perpetua"/>
+        <family val="1"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Perpetua"/>
+        <family val="1"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Perpetua"/>
+        <family val="1"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Perpetua"/>
+        <family val="1"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Perpetua"/>
+        <family val="1"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -657,13 +711,13 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="To-do list for projects">
     <tableStyle name="To-do list for projects" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="10"/>
-      <tableStyleElement type="headerRow" dxfId="9"/>
-      <tableStyleElement type="totalRow" dxfId="8"/>
-      <tableStyleElement type="firstColumn" dxfId="7"/>
-      <tableStyleElement type="lastColumn" dxfId="6"/>
-      <tableStyleElement type="firstRowStripe" dxfId="5"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="4"/>
+      <tableStyleElement type="wholeTable" dxfId="22"/>
+      <tableStyleElement type="headerRow" dxfId="21"/>
+      <tableStyleElement type="totalRow" dxfId="20"/>
+      <tableStyleElement type="firstColumn" dxfId="19"/>
+      <tableStyleElement type="lastColumn" dxfId="18"/>
+      <tableStyleElement type="firstRowStripe" dxfId="17"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="16"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -677,16 +731,20 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4076D023-3123-4435-9B03-717B351FB214}" name="Project167" displayName="Project167" ref="B7:H14" totalsRowShown="0">
-  <autoFilter ref="B7:H14" xr:uid="{A46E5AE3-66B6-48F2-9036-DC0EC84EE724}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4076D023-3123-4435-9B03-717B351FB214}" name="Project167" displayName="Project167" ref="B7:H15" totalsRowShown="0">
+  <autoFilter ref="B7:H15" xr:uid="{A46E5AE3-66B6-48F2-9036-DC0EC84EE724}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{52333874-C2BC-4FBF-9AA5-5291ED527120}" name="% done" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{52333874-C2BC-4FBF-9AA5-5291ED527120}" name="% done" dataDxfId="4" dataCellStyle="Percent"/>
     <tableColumn id="2" xr3:uid="{B01D3C54-85C7-4AC4-B550-F441F081A8E7}" name="Phase" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{4A96FAF1-6CFF-4C95-A1B9-D6A409D17E24}" name="Start By"/>
-    <tableColumn id="7" xr3:uid="{288AAF48-94FD-483E-BC80-43361A2172AA}" name="Original Due By"/>
-    <tableColumn id="3" xr3:uid="{079E2D1B-453B-4EE7-A63C-A52ADC49D9FF}" name="Revised Due By" dataCellStyle="Date"/>
-    <tableColumn id="8" xr3:uid="{391FA284-95B3-4A59-A408-B42F0990F555}" name="Number Of Days" dataDxfId="3" dataCellStyle="Date"/>
+    <tableColumn id="5" xr3:uid="{4A96FAF1-6CFF-4C95-A1B9-D6A409D17E24}" name="Start By" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{288AAF48-94FD-483E-BC80-43361A2172AA}" name="Original Due By" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{079E2D1B-453B-4EE7-A63C-A52ADC49D9FF}" name="Revised Due By" dataDxfId="1" dataCellStyle="Date"/>
+    <tableColumn id="8" xr3:uid="{391FA284-95B3-4A59-A408-B42F0990F555}" name="Number Of Days" dataDxfId="0" dataCellStyle="Date"/>
     <tableColumn id="4" xr3:uid="{3331DA69-AA66-4458-9EB4-B030D208F716}" name="Revision Notes"/>
   </tableColumns>
   <tableStyleInfo name="To-do list for projects" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -702,12 +760,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{242FB2F3-2A5C-4306-BA9C-4FA89A4B88A2}" name="Project1679" displayName="Project1679" ref="B7:H15" totalsRowShown="0">
   <autoFilter ref="B7:H15" xr:uid="{EFE520EF-21FC-4315-9A01-F23FD8E516E3}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D8DCF90F-A23E-49B6-A47F-34297985A49C}" name="% done" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{D8DCF90F-A23E-49B6-A47F-34297985A49C}" name="% done" dataDxfId="9" dataCellStyle="Percent"/>
     <tableColumn id="2" xr3:uid="{CF26B0BB-5B4E-4253-94AB-D0FF97C1EFAD}" name="Phase" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{0F9A5899-431E-43E9-917D-A7AEE008B96C}" name="Start By"/>
-    <tableColumn id="7" xr3:uid="{3901E6BC-3146-4763-BD50-C73630D73D01}" name="Original Due By"/>
-    <tableColumn id="3" xr3:uid="{BEFADCA8-D174-47F6-9028-257FEFDAEB18}" name="Revised Due By" dataCellStyle="Date"/>
-    <tableColumn id="8" xr3:uid="{924D9BAB-2A88-4987-AF70-68B3B9645206}" name="Number Of Days" dataDxfId="2" dataCellStyle="Date"/>
+    <tableColumn id="5" xr3:uid="{0F9A5899-431E-43E9-917D-A7AEE008B96C}" name="Start By" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{3901E6BC-3146-4763-BD50-C73630D73D01}" name="Original Due By" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{BEFADCA8-D174-47F6-9028-257FEFDAEB18}" name="Revised Due By" dataDxfId="6" dataCellStyle="Date"/>
+    <tableColumn id="8" xr3:uid="{924D9BAB-2A88-4987-AF70-68B3B9645206}" name="Number Of Days" dataDxfId="5" dataCellStyle="Date"/>
     <tableColumn id="4" xr3:uid="{B690C0A8-6088-4AAA-911C-D12BBC6A687D}" name="Revision Notes"/>
   </tableColumns>
   <tableStyleInfo name="To-do list for projects" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -723,12 +781,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{07EB7E31-9571-48EE-8CF4-A2823DE4A9D0}" name="Project16710" displayName="Project16710" ref="B7:H15" totalsRowShown="0">
   <autoFilter ref="B7:H15" xr:uid="{59B5756C-FDEF-4839-A78B-1F56E2D0B4CD}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9C97606B-E575-415C-B47A-7AD57C400FE5}" name="% done" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{9C97606B-E575-415C-B47A-7AD57C400FE5}" name="% done" dataDxfId="14" dataCellStyle="Percent"/>
     <tableColumn id="2" xr3:uid="{CB80D31A-7130-42B6-90AE-85A55AA25E8D}" name="Phase" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{AC33B8ED-8BF0-44AC-8A68-889CA8686F8E}" name="Start By"/>
-    <tableColumn id="7" xr3:uid="{353DA3C8-FC50-4AE0-B68B-653CFF7B021C}" name="Original Due By"/>
-    <tableColumn id="3" xr3:uid="{383F117A-00AF-4025-A5FA-BE3DB143B37C}" name="Revised Due By" dataCellStyle="Date"/>
-    <tableColumn id="8" xr3:uid="{FC169D18-5326-465B-AC22-AAE3DAD8776D}" name="Number Of Days" dataDxfId="1" dataCellStyle="Date"/>
+    <tableColumn id="5" xr3:uid="{AC33B8ED-8BF0-44AC-8A68-889CA8686F8E}" name="Start By" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{353DA3C8-FC50-4AE0-B68B-653CFF7B021C}" name="Original Due By" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{383F117A-00AF-4025-A5FA-BE3DB143B37C}" name="Revised Due By" dataDxfId="11" dataCellStyle="Date"/>
+    <tableColumn id="8" xr3:uid="{FC169D18-5326-465B-AC22-AAE3DAD8776D}" name="Number Of Days" dataDxfId="10" dataCellStyle="Date"/>
     <tableColumn id="4" xr3:uid="{F626FC71-D9D6-4F16-9F1D-68AB655AFB4F}" name="Revision Notes"/>
   </tableColumns>
   <tableStyleInfo name="To-do list for projects" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -749,7 +807,7 @@
     <tableColumn id="5" xr3:uid="{975EBC13-24BD-4728-A8EC-9D2F06633F32}" name="Start By"/>
     <tableColumn id="7" xr3:uid="{A45F7DEE-3414-42C2-965F-B963467B1743}" name="Original Due By2"/>
     <tableColumn id="3" xr3:uid="{AE79D1E6-B560-422E-BC0A-E4F69D3AD679}" name="Revised Due By" dataCellStyle="Date"/>
-    <tableColumn id="8" xr3:uid="{6A477119-15D5-41F0-BF23-60DAD5ECB7D6}" name="Number Of Days" dataDxfId="0" dataCellStyle="Date"/>
+    <tableColumn id="8" xr3:uid="{6A477119-15D5-41F0-BF23-60DAD5ECB7D6}" name="Number Of Days" dataDxfId="15" dataCellStyle="Date"/>
     <tableColumn id="4" xr3:uid="{595BD41C-7869-4A83-9894-71F2EEA27F12}" name="Revision Notes"/>
   </tableColumns>
   <tableStyleInfo name="To-do list for projects" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1109,10 +1167,10 @@
     <tabColor theme="5" tint="0.79998168889431442"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H16"/>
+  <dimension ref="B1:H17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1141,64 +1199,64 @@
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9"/>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
+      <c r="F3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="15"/>
+      <c r="F4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>12</v>
-      </c>
-      <c r="H7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1209,19 +1267,19 @@
         <v>4</v>
       </c>
       <c r="D8" s="6">
-        <v>45943</v>
+        <v>46001</v>
       </c>
       <c r="E8" s="6">
-        <v>45944</v>
+        <v>46004</v>
       </c>
       <c r="F8" s="4">
-        <v>45944</v>
+        <v>46004</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1232,19 +1290,19 @@
         <v>5</v>
       </c>
       <c r="D9" s="6">
-        <v>45944</v>
+        <v>46002</v>
       </c>
       <c r="E9" s="6">
-        <v>45944</v>
+        <v>46004</v>
       </c>
       <c r="F9" s="4">
-        <v>45944</v>
+        <v>46004</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>61</v>
+        <v>18</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1252,40 +1310,42 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="7">
-        <v>45944</v>
+        <v>20</v>
+      </c>
+      <c r="D10" s="6">
+        <v>46005</v>
       </c>
       <c r="E10" s="6">
-        <v>45945</v>
+        <v>46005</v>
       </c>
       <c r="F10" s="4">
-        <v>45946</v>
+        <v>46005</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10"/>
+        <v>19</v>
+      </c>
+      <c r="H10" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="11" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="6">
-        <v>45945</v>
+        <v>46005</v>
       </c>
       <c r="E11" s="6">
-        <v>45945</v>
+        <v>46005</v>
       </c>
       <c r="F11" s="4">
-        <v>45946</v>
+        <v>46005</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H11"/>
     </row>
@@ -1294,22 +1354,22 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="6">
-        <v>45946</v>
+        <v>46006</v>
       </c>
       <c r="E12" s="6">
-        <v>45946</v>
+        <v>46006</v>
       </c>
       <c r="F12" s="4">
-        <v>45946</v>
+        <v>46006</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1317,20 +1377,22 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="D13" s="6">
-        <v>45946</v>
+        <v>46006</v>
       </c>
       <c r="E13" s="6">
-        <v>45946</v>
+        <v>46006</v>
       </c>
       <c r="F13" s="4">
-        <v>45946</v>
-      </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="1" t="s">
-        <v>45</v>
+        <v>46006</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1341,38 +1403,55 @@
         <v>25</v>
       </c>
       <c r="D14" s="6">
-        <v>45946</v>
+        <v>46007</v>
       </c>
       <c r="E14" s="6">
-        <v>45946</v>
+        <v>46007</v>
       </c>
       <c r="F14" s="4">
-        <v>45946</v>
+        <v>46007</v>
       </c>
       <c r="G14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="3"/>
-      <c r="C15"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15"/>
+      <c r="D15" s="6">
+        <v>46007</v>
+      </c>
+      <c r="E15" s="6">
+        <v>46007</v>
+      </c>
+      <c r="F15" s="4">
+        <v>46007</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="16" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="3"/>
       <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
       <c r="H16"/>
+    </row>
+    <row r="17" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1382,8 +1461,17 @@
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="B6:H6"/>
   </mergeCells>
-  <conditionalFormatting sqref="B8:B16">
-    <cfRule type="dataBar" priority="7">
+  <conditionalFormatting sqref="B16:B17">
+    <cfRule type="dataBar" priority="11">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF92D050"/>
+      </dataBar>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:B15">
+    <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1423,8 +1511,8 @@
   </sheetPr>
   <dimension ref="B1:H16"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B12" zoomScale="65" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="65" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1450,64 +1538,64 @@
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9"/>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
+      <c r="F3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="15"/>
+      <c r="F4" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>12</v>
-      </c>
-      <c r="H7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1515,177 +1603,181 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="D8" s="6">
-        <v>45943</v>
+        <v>46001</v>
       </c>
       <c r="E8" s="6">
-        <v>45944</v>
+        <v>46004</v>
       </c>
       <c r="F8" s="4">
-        <v>45944</v>
+        <v>46004</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
         <v>27</v>
       </c>
-      <c r="H8"/>
     </row>
     <row r="9" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="3">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="7">
-        <v>45943</v>
+        <v>5</v>
+      </c>
+      <c r="D9" s="6">
+        <v>46002</v>
       </c>
       <c r="E9" s="6">
-        <v>45943</v>
+        <v>46004</v>
       </c>
       <c r="F9" s="4">
-        <v>45943</v>
+        <v>46004</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D10" s="6">
-        <v>45944</v>
+        <v>46005</v>
       </c>
       <c r="E10" s="6">
-        <v>45944</v>
+        <v>46005</v>
       </c>
       <c r="F10" s="4">
-        <v>45945</v>
+        <v>46005</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10"/>
+        <v>19</v>
+      </c>
+      <c r="H10" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="11" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D11" s="6">
-        <v>45945</v>
+        <v>46005</v>
       </c>
       <c r="E11" s="6">
-        <v>45945</v>
+        <v>46005</v>
       </c>
       <c r="F11" s="4">
-        <v>45945</v>
+        <v>46005</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="H11"/>
     </row>
     <row r="12" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D12" s="6">
-        <v>45946</v>
+        <v>46006</v>
       </c>
       <c r="E12" s="6">
-        <v>45946</v>
+        <v>46006</v>
       </c>
       <c r="F12" s="4">
-        <v>45946</v>
+        <v>46006</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="H12" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D13" s="6">
-        <v>45946</v>
+        <v>46006</v>
       </c>
       <c r="E13" s="6">
-        <v>45946</v>
+        <v>46006</v>
       </c>
       <c r="F13" s="4">
-        <v>45946</v>
+        <v>46006</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>63</v>
+        <v>19</v>
+      </c>
+      <c r="H13" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D14" s="6">
-        <v>45946</v>
+        <v>46007</v>
       </c>
       <c r="E14" s="6">
-        <v>45946</v>
+        <v>46007</v>
       </c>
       <c r="F14" s="4">
-        <v>45946</v>
+        <v>46007</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="H14" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D15" s="6">
-        <v>45946</v>
+        <v>46007</v>
       </c>
       <c r="E15" s="6">
-        <v>45947</v>
+        <v>46007</v>
       </c>
       <c r="F15" s="4">
-        <v>45947</v>
+        <v>46007</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H15" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1706,7 +1798,7 @@
     <mergeCell ref="B6:H6"/>
   </mergeCells>
   <conditionalFormatting sqref="B8:B15">
-    <cfRule type="dataBar" priority="8">
+    <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1746,8 +1838,8 @@
   </sheetPr>
   <dimension ref="B1:H16"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A9" zoomScale="69" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView showGridLines="0" zoomScale="69" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1773,64 +1865,64 @@
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9"/>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
+      <c r="F3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="15"/>
+      <c r="F4" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>12</v>
-      </c>
-      <c r="H7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1838,177 +1930,181 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="D8" s="6">
-        <v>45943</v>
+        <v>46001</v>
       </c>
       <c r="E8" s="6">
-        <v>45944</v>
+        <v>46004</v>
       </c>
       <c r="F8" s="4">
-        <v>45944</v>
+        <v>46004</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H8" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="3">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="D9" s="6">
-        <v>45944</v>
+        <v>46002</v>
       </c>
       <c r="E9" s="6">
-        <v>45944</v>
+        <v>46004</v>
       </c>
       <c r="F9" s="4">
-        <v>45944</v>
+        <v>46004</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D10" s="6">
-        <v>45944</v>
+        <v>46005</v>
       </c>
       <c r="E10" s="6">
-        <v>45944</v>
+        <v>46005</v>
       </c>
       <c r="F10" s="4">
-        <v>45944</v>
+        <v>46005</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D11" s="6">
-        <v>45944</v>
+        <v>46005</v>
       </c>
       <c r="E11" s="6">
-        <v>45945</v>
+        <v>46005</v>
       </c>
       <c r="F11" s="4">
-        <v>45946</v>
+        <v>46005</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="H11"/>
     </row>
     <row r="12" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D12" s="6">
-        <v>45945</v>
+        <v>46006</v>
       </c>
       <c r="E12" s="6">
-        <v>45945</v>
+        <v>46006</v>
       </c>
       <c r="F12" s="4">
-        <v>45946</v>
+        <v>46006</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12"/>
+        <v>19</v>
+      </c>
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="6">
-        <v>45946</v>
+        <v>46006</v>
       </c>
       <c r="E13" s="6">
-        <v>45946</v>
+        <v>46006</v>
       </c>
       <c r="F13" s="4">
-        <v>45946</v>
+        <v>46006</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D14" s="6">
-        <v>45946</v>
+        <v>46007</v>
       </c>
       <c r="E14" s="6">
-        <v>45946</v>
+        <v>46007</v>
       </c>
       <c r="F14" s="4">
-        <v>45947</v>
+        <v>46007</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14"/>
+        <v>19</v>
+      </c>
+      <c r="H14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D15" s="6">
-        <v>45946</v>
+        <v>46007</v>
       </c>
       <c r="E15" s="6">
-        <v>45947</v>
+        <v>46007</v>
       </c>
       <c r="F15" s="4">
-        <v>45947</v>
+        <v>46007</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H15" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2029,7 +2125,7 @@
     <mergeCell ref="B6:H6"/>
   </mergeCells>
   <conditionalFormatting sqref="B8:B15">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2065,8 +2161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30E5B4F-2070-4E52-85B8-76686C2B4348}">
   <dimension ref="B1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="B8:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2094,64 +2190,64 @@
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9"/>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
+      <c r="F3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="2:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="15"/>
+      <c r="F4" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>12</v>
-      </c>
-      <c r="H7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2171,10 +2267,10 @@
         <v>46004</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H8" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2194,10 +2290,10 @@
         <v>46004</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2205,7 +2301,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D10" s="6">
         <v>46005</v>
@@ -2217,10 +2313,10 @@
         <v>46005</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2228,7 +2324,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D11" s="6">
         <v>46005</v>
@@ -2240,7 +2336,7 @@
         <v>46005</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H11"/>
     </row>
@@ -2249,7 +2345,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D12" s="6">
         <v>46006</v>
@@ -2261,10 +2357,10 @@
         <v>46006</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H12" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2272,7 +2368,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D13" s="6">
         <v>46006</v>
@@ -2284,10 +2380,10 @@
         <v>46006</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2295,7 +2391,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D14" s="6">
         <v>46007</v>
@@ -2307,10 +2403,10 @@
         <v>46007</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H14" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -2318,7 +2414,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D15" s="6">
         <v>46007</v>
@@ -2330,10 +2426,10 @@
         <v>46007</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H15" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>